<commit_message>
additions to feature tables
</commit_message>
<xml_diff>
--- a/features/LanguageWorkbench_FeatureConfiguration.xlsx
+++ b/features/LanguageWorkbench_FeatureConfiguration.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="175">
   <si>
     <t xml:space="preserve">Feature</t>
   </si>
@@ -46,6 +46,9 @@
     <t xml:space="preserve">│   │   └── Define good practices</t>
   </si>
   <si>
+    <t xml:space="preserve">not supported</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   ├── Syntax Definition</t>
   </si>
   <si>
@@ -58,9 +61,6 @@
     <t xml:space="preserve">│   │   │   ├── AS from examples</t>
   </si>
   <si>
-    <t xml:space="preserve">not supported</t>
-  </si>
-  <si>
     <t xml:space="preserve">│   │   │   └── AS from scratch</t>
   </si>
   <si>
@@ -154,6 +154,9 @@
     <t xml:space="preserve">│   │   │   │   ├── Model of communication</t>
   </si>
   <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   │   │   │   └── Model of concurrency</t>
   </si>
   <si>
@@ -187,9 +190,15 @@
     <t xml:space="preserve">│   │   ├── MW Highlighting</t>
   </si>
   <si>
+    <t xml:space="preserve">through textX-LS LSP server/client</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   │   ├── MW Folding</t>
   </si>
   <si>
+    <t xml:space="preserve">generic offered by VS Code</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   │   ├── MW Syntactic completion</t>
   </si>
   <si>
@@ -223,6 +232,9 @@
     <t xml:space="preserve">│   │   │   └── Programmatic</t>
   </si>
   <si>
+    <t xml:space="preserve">in Python</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   │   ├── Formal verification</t>
   </si>
   <si>
@@ -238,6 +250,9 @@
     <t xml:space="preserve">│   │   ├── MW debugger</t>
   </si>
   <si>
+    <t xml:space="preserve">Python debugger is used</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   │   │   └── Omniscient debugger</t>
   </si>
   <si>
@@ -367,15 +382,15 @@
     <t xml:space="preserve">│   │   └── Declarative</t>
   </si>
   <si>
+    <t xml:space="preserve">grammar</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   ├── Artifact</t>
   </si>
   <si>
     <t xml:space="preserve">│   │   ├── Model-based</t>
   </si>
   <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
     <t xml:space="preserve">│   │   ├── Grammar-based</t>
   </si>
   <si>
@@ -448,6 +463,9 @@
     <t xml:space="preserve">│   │   │   ├── Optimistic</t>
   </si>
   <si>
+    <t xml:space="preserve">Through text-based VCS</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   │   │   └── Pessimistic</t>
   </si>
   <si>
@@ -457,9 +475,15 @@
     <t xml:space="preserve">│   │   │   ├── Distributed</t>
   </si>
   <si>
+    <t xml:space="preserve">Through text-based VCS(Git, Mercurial…)</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   │   │   └── Centralized</t>
   </si>
   <si>
+    <t xml:space="preserve">Through text-based VCS(Subversion)</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   └── Versioning</t>
   </si>
   <si>
@@ -472,12 +496,21 @@
     <t xml:space="preserve">│   │   ├── Desktop</t>
   </si>
   <si>
+    <t xml:space="preserve">TextX-LS editor, solution can be deployed to any Python environment</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   │   └── Cloud-native</t>
   </si>
   <si>
+    <t xml:space="preserve">Althoug, solutions can be deployed to any Python environment</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   └── Modular</t>
   </si>
   <si>
+    <t xml:space="preserve">languages/generators can be separate Python packages, dynamic discovery</t>
+  </si>
+  <si>
     <t xml:space="preserve">├── MW production</t>
   </si>
   <si>
@@ -487,7 +520,13 @@
     <t xml:space="preserve">│   │   ├── Generation</t>
   </si>
   <si>
+    <t xml:space="preserve">can use any template-engine (Jinja2 is supported through textx-jinja project)</t>
+  </si>
+  <si>
     <t xml:space="preserve">│   │   └── Interpretation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interpreter defined in Python</t>
   </si>
   <si>
     <t xml:space="preserve">│   └── Continuous production</t>
@@ -901,15 +940,15 @@
   </sheetPr>
   <dimension ref="A1:F145"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A96" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B117" activeCellId="0" sqref="B117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.59765625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="54.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="47.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="47.37"/>
   </cols>
@@ -962,10 +1001,13 @@
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -976,7 +1018,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
@@ -985,16 +1027,16 @@
         <v>4</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
@@ -1036,10 +1078,10 @@
         <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F11" s="9"/>
     </row>
@@ -1089,7 +1131,7 @@
         <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1097,7 +1139,7 @@
         <v>27</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,7 +1147,7 @@
         <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1132,7 +1174,7 @@
         <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1206,7 +1248,7 @@
         <v>39</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,15 +1271,21 @@
       <c r="A31" s="3" t="s">
         <v>43</v>
       </c>
+      <c r="B31" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>4</v>
@@ -1248,17 +1296,29 @@
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>4</v>
@@ -1269,22 +1329,31 @@
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>4</v>
@@ -1295,7 +1364,7 @@
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>4</v>
@@ -1306,27 +1375,48 @@
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="3" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>4</v>
@@ -1337,17 +1427,23 @@
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="3" t="s">
-        <v>59</v>
+        <v>62</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>4</v>
@@ -1358,12 +1454,12 @@
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>4</v>
@@ -1374,37 +1470,58 @@
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>4</v>
@@ -1415,17 +1532,29 @@
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3" t="s">
-        <v>72</v>
+        <v>77</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>4</v>
@@ -1436,7 +1565,7 @@
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>4</v>
@@ -1447,7 +1576,7 @@
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>16</v>
@@ -1455,23 +1584,23 @@
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="3" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="3" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>4</v>
@@ -1482,58 +1611,64 @@
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="3" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="3" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="3" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="3" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="3" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>4</v>
@@ -1544,31 +1679,31 @@
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="3" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="3" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="3" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>16</v>
@@ -1576,31 +1711,31 @@
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="3" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="3" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>4</v>
@@ -1611,23 +1746,23 @@
     </row>
     <row r="82" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="3" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="3" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>4</v>
@@ -1638,7 +1773,7 @@
     </row>
     <row r="85" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="3" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>4</v>
@@ -1649,7 +1784,7 @@
     </row>
     <row r="86" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="3" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>16</v>
@@ -1657,55 +1792,55 @@
     </row>
     <row r="87" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="3" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="3" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="3" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="3" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="3" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>4</v>
@@ -1716,7 +1851,7 @@
     </row>
     <row r="94" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="3" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>4</v>
@@ -1727,31 +1862,31 @@
     </row>
     <row r="95" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="3" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="3" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="3" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="3" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>16</v>
@@ -1759,7 +1894,7 @@
     </row>
     <row r="99" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="3" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>4</v>
@@ -1770,17 +1905,26 @@
     </row>
     <row r="100" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="3" t="s">
-        <v>113</v>
+        <v>118</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="3" t="s">
-        <v>114</v>
+        <v>119</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="3" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>4</v>
@@ -1791,34 +1935,31 @@
     </row>
     <row r="103" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="3" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>117</v>
+        <v>8</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>117</v>
-      </c>
     </row>
     <row r="105" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="3" t="s">
-        <v>119</v>
+        <v>124</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="3" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>4</v>
@@ -1829,40 +1970,40 @@
     </row>
     <row r="107" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="3" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="3" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="3" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>4</v>
@@ -1873,7 +2014,7 @@
     </row>
     <row r="111" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="3" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>4</v>
@@ -1884,33 +2025,33 @@
     </row>
     <row r="112" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="3" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="3" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="3" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="3" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="3" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>4</v>
@@ -1921,32 +2062,32 @@
     </row>
     <row r="117" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="3" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="3" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="3" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="3" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="3" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="3" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>4</v>
@@ -1957,7 +2098,7 @@
     </row>
     <row r="123" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="3" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>4</v>
@@ -1968,7 +2109,7 @@
     </row>
     <row r="124" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="3" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>4</v>
@@ -1979,17 +2120,29 @@
     </row>
     <row r="125" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="3" t="s">
-        <v>141</v>
+        <v>146</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="3" t="s">
-        <v>142</v>
+        <v>148</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="3" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>4</v>
@@ -2000,22 +2153,40 @@
     </row>
     <row r="128" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="3" t="s">
-        <v>144</v>
+        <v>150</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="3" t="s">
-        <v>145</v>
+        <v>152</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="3" t="s">
-        <v>146</v>
+        <v>154</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="3" t="s">
-        <v>147</v>
+        <v>155</v>
       </c>
       <c r="B131" s="2" t="s">
         <v>4</v>
@@ -2026,7 +2197,7 @@
     </row>
     <row r="132" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="3" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>4</v>
@@ -2037,22 +2208,40 @@
     </row>
     <row r="133" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="3" t="s">
-        <v>149</v>
+        <v>157</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="3" t="s">
-        <v>150</v>
+        <v>159</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="3" t="s">
-        <v>151</v>
+        <v>161</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="3" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>4</v>
@@ -2063,7 +2252,7 @@
     </row>
     <row r="137" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="3" t="s">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>4</v>
@@ -2074,22 +2263,37 @@
     </row>
     <row r="138" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="3" t="s">
-        <v>154</v>
+        <v>165</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="3" t="s">
-        <v>155</v>
+        <v>167</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="3" t="s">
-        <v>156</v>
+        <v>169</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="3" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>4</v>
@@ -2100,34 +2304,34 @@
     </row>
     <row r="142" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="3" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="3" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="3" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="3" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>